<commit_message>
Rajout debut word benchmark techno + méthode
</commit_message>
<xml_diff>
--- a/rapports/Comparatif méthodes.xlsx
+++ b/rapports/Comparatif méthodes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="133">
   <si>
     <t>Thème</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Balises ultrasons                                   2 équipes : uart et l'ESEO</t>
+  </si>
+  <si>
+    <t>Possibilité d'utiliser des capteurs industriels</t>
+  </si>
+  <si>
+    <t>A voir</t>
   </si>
 </sst>
 </file>
@@ -724,13 +730,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,18 +740,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -791,6 +779,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1091,11 +1097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1109,567 +1115,602 @@
     <col min="7" max="7" width="23.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="3"/>
-    <col min="11" max="11" width="21.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="3" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" style="3"/>
+    <col min="12" max="12" width="21.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:13" ht="75.75" thickBot="1">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="M2" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="60.75" thickBot="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="22"/>
+      <c r="B4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="M4" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="60.75" thickBot="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:13" ht="45" customHeight="1">
+      <c r="A6" s="22"/>
+      <c r="B6" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="19" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="M6" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="135.75" thickBot="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="8" t="s">
+    <row r="7" spans="1:13" ht="135.75" thickBot="1">
+      <c r="A7" s="22"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>66</v>
       </c>
       <c r="J7"/>
-      <c r="K7" s="8" t="s">
+      <c r="K7"/>
+      <c r="L7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="11"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="22"/>
+      <c r="B8" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="M8" s="20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="69.75" customHeight="1" thickBot="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="8" t="s">
+    <row r="9" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
+      <c r="A9" s="23"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="6" t="s">
         <v>105</v>
       </c>
       <c r="J9"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="9" t="s">
+      <c r="K9"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="M10" s="20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="90.75" thickBot="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8" t="s">
+    <row r="11" spans="1:13" ht="90.75" thickBot="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="6" t="s">
         <v>77</v>
       </c>
       <c r="J11"/>
-      <c r="K11" s="8" t="s">
+      <c r="K11"/>
+      <c r="L11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="M11" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:13">
+      <c r="A12" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="M12" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="75.75" thickBot="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+    <row r="13" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="M13" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:13" ht="45" customHeight="1">
+      <c r="A14" s="22"/>
+      <c r="B14" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="26" t="s">
+      <c r="M14" s="20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
+    <row r="15" spans="1:13" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A15" s="22"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="11"/>
-      <c r="B16" s="4" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="22"/>
+      <c r="B16" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="22" t="s">
+      <c r="E16" s="13"/>
+      <c r="F16" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="M16" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="60.75" thickBot="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="8" t="s">
+    <row r="17" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A17" s="23"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="M17" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1688,14 +1729,6 @@
     <mergeCell ref="A2:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="E2 E4 E8 E12 E14">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1704,6 +1737,14 @@
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1719,7 +1760,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:L2">
+  <conditionalFormatting sqref="C2:M2">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2041,7 +2082,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="I21">
-        <f t="shared" ref="I20:I22" si="1">$I$2-$B$18</f>
+        <f t="shared" ref="I21" si="1">$I$2-$B$18</f>
         <v>79</v>
       </c>
       <c r="J21">
@@ -2055,7 +2096,7 @@
         <v>101</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J20:J22" si="2">$J$2-$B$18</f>
+        <f t="shared" ref="J22" si="2">$J$2-$B$18</f>
         <v>34</v>
       </c>
     </row>
@@ -2243,7 +2284,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="I37">
-        <f t="shared" ref="I36:I38" si="4">$I$2-$B$34</f>
+        <f t="shared" ref="I37" si="4">$I$2-$B$34</f>
         <v>89.5</v>
       </c>
       <c r="J37">
@@ -2257,7 +2298,7 @@
         <v>90.5</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J36:J38" si="5">$J$2-$B$34</f>
+        <f t="shared" ref="J38" si="5">$J$2-$B$34</f>
         <v>44.5</v>
       </c>
     </row>
@@ -2445,7 +2486,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="I53">
-        <f t="shared" ref="I52:I54" si="7">$I$2-$B$50</f>
+        <f t="shared" ref="I53" si="7">$I$2-$B$50</f>
         <v>89.9</v>
       </c>
       <c r="J53">
@@ -2459,7 +2500,7 @@
         <v>90.1</v>
       </c>
       <c r="J54">
-        <f t="shared" ref="J52:J54" si="8">$J$2-$B$50</f>
+        <f t="shared" ref="J54" si="8">$J$2-$B$50</f>
         <v>44.9</v>
       </c>
     </row>

</xml_diff>